<commit_message>
replaced project files with the commented and refactored version along with bash file to automate the compression, decompression process
</commit_message>
<xml_diff>
--- a/Compressor Decompressor Results.xlsx
+++ b/Compressor Decompressor Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fiea\sem1\Programming 1\C Comressor Decompressor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fiea\sem1\Programming 1\NJ Zip\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>No. of Bits</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>File Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of Original Data File = </t>
   </si>
 </sst>
 </file>
@@ -76,9 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,8 +421,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="437759376"/>
-        <c:axId val="437759768"/>
+        <c:axId val="207770288"/>
+        <c:axId val="207764408"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -506,16 +510,72 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="437758984"/>
-        <c:axId val="437752712"/>
+        <c:axId val="207762840"/>
+        <c:axId val="207769896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="437759376"/>
+        <c:axId val="207770288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. Of Compression Bits</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -553,7 +613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437759768"/>
+        <c:crossAx val="207764408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -561,7 +621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437759768"/>
+        <c:axId val="207764408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,6 +641,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>File Size (in Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -612,17 +728,78 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437759376"/>
+        <c:crossAx val="207770288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="437752712"/>
+        <c:axId val="207769896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Root</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Mean Sq. Error</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -654,13 +831,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437758984"/>
+        <c:crossAx val="207762840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1.0000000000000002E-3"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="437758984"/>
+        <c:axId val="207762840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +846,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="437752712"/>
+        <c:crossAx val="207769896"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1313,15 +1491,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1606,20 +1784,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1629,8 +1808,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2">
+        <v>286549</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1641,7 +1827,7 @@
         <v>6722</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1652,7 +1838,7 @@
         <v>8062</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -1663,7 +1849,7 @@
         <v>9401</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1674,7 +1860,7 @@
         <v>10741</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1685,7 +1871,7 @@
         <v>12080</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1696,7 +1882,7 @@
         <v>13420</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -1707,7 +1893,7 @@
         <v>14759</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1718,7 +1904,7 @@
         <v>16099</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13</v>
       </c>
@@ -1729,7 +1915,7 @@
         <v>17438</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
@@ -1740,7 +1926,7 @@
         <v>18778</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -1751,7 +1937,7 @@
         <v>20117</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>

</xml_diff>